<commit_message>
add uploaded Excel rows to ImportPlayersPage
</commit_message>
<xml_diff>
--- a/static/import_players_template.xlsx
+++ b/static/import_players_template.xlsx
@@ -167,48 +167,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <fill>
         <patternFill>
@@ -222,6 +203,64 @@
           <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -234,24 +273,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O30" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O30" totalsRowShown="0" dataDxfId="2">
   <autoFilter ref="A1:O30"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Nationality"/>
-    <tableColumn id="3" name="Position"/>
-    <tableColumn id="4" name="Secondary Position(s)"/>
-    <tableColumn id="5" name="Age" dataDxfId="9"/>
-    <tableColumn id="6" name="OVR" dataDxfId="8"/>
-    <tableColumn id="7" name="Value" dataDxfId="7"/>
-    <tableColumn id="8" name="Kit Number" dataDxfId="6"/>
-    <tableColumn id="9" name="Contract Ends" dataDxfId="5"/>
-    <tableColumn id="10" name="Wage" dataDxfId="4" dataCellStyle="Currency"/>
-    <tableColumn id="11" name="Signing Bonus" dataDxfId="3" dataCellStyle="Currency"/>
-    <tableColumn id="12" name="Release Clause" dataDxfId="2" dataCellStyle="Currency"/>
-    <tableColumn id="13" name="Performance Bonus" dataDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="14" name="Bonus Req" dataDxfId="0"/>
-    <tableColumn id="15" name="Bonus Req. Type"/>
+    <tableColumn id="1" name="Name" dataDxfId="17"/>
+    <tableColumn id="2" name="Nationality" dataDxfId="16"/>
+    <tableColumn id="3" name="Position" dataDxfId="15"/>
+    <tableColumn id="4" name="Secondary Position(s)" dataDxfId="14"/>
+    <tableColumn id="5" name="Age" dataDxfId="13"/>
+    <tableColumn id="6" name="OVR" dataDxfId="12"/>
+    <tableColumn id="7" name="Value" dataDxfId="11"/>
+    <tableColumn id="8" name="Kit Number" dataDxfId="10"/>
+    <tableColumn id="9" name="Contract Ends" dataDxfId="9"/>
+    <tableColumn id="10" name="Wage" dataDxfId="8" dataCellStyle="Currency"/>
+    <tableColumn id="11" name="Signing Bonus" dataDxfId="7" dataCellStyle="Currency"/>
+    <tableColumn id="12" name="Release Clause" dataDxfId="6" dataCellStyle="Currency"/>
+    <tableColumn id="13" name="Performance Bonus" dataDxfId="5" dataCellStyle="Currency"/>
+    <tableColumn id="14" name="Bonus Req" dataDxfId="4"/>
+    <tableColumn id="15" name="Bonus Req. Type" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -581,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -591,6 +630,7 @@
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.75" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.75" customWidth="1"/>
@@ -649,361 +689,507 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="4"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
       <c r="N2" s="2"/>
+      <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="4"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
       <c r="N3" s="2"/>
+      <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
       <c r="N4" s="2"/>
+      <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
       <c r="N5" s="2"/>
+      <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
       <c r="N6" s="2"/>
+      <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
       <c r="N7" s="2"/>
+      <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
       <c r="N8" s="2"/>
+      <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
       <c r="N9" s="2"/>
+      <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="4"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
       <c r="N10" s="2"/>
+      <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="4"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
       <c r="N11" s="2"/>
+      <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="4"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
       <c r="N12" s="2"/>
+      <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
       <c r="N13" s="2"/>
+      <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="3"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
       <c r="N14" s="2"/>
+      <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
       <c r="N15" s="2"/>
+      <c r="O15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
       <c r="N16" s="2"/>
-    </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="4"/>
+      <c r="G17" s="3"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
       <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="3"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
       <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
       <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="4"/>
+      <c r="G20" s="3"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
       <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="4"/>
+      <c r="G21" s="3"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
       <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="4"/>
+      <c r="G22" s="3"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
       <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="4"/>
+      <c r="G23" s="3"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
       <c r="N23" s="2"/>
-    </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="4"/>
+      <c r="G24" s="3"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
       <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="4"/>
+      <c r="G25" s="3"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
       <c r="N25" s="2"/>
-    </row>
-    <row r="26" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="4"/>
+      <c r="G26" s="3"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
       <c r="N26" s="2"/>
-    </row>
-    <row r="27" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="4"/>
+      <c r="G27" s="3"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
       <c r="N27" s="2"/>
-    </row>
-    <row r="28" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="4"/>
+      <c r="G28" s="3"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
       <c r="N28" s="2"/>
-    </row>
-    <row r="29" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="4"/>
+      <c r="G29" s="3"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
       <c r="N29" s="2"/>
-    </row>
-    <row r="30" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="4"/>
+      <c r="G30" s="3"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
       <c r="N30" s="2"/>
+      <c r="O30" s="1"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
   <conditionalFormatting sqref="N2:O2">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>ISBLANK($M2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:O30">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>ISBLANK($M3)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>